<commit_message>
add pcs for spare parts, same rafractoring
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/template.xlsx
+++ b/eq_log/eq_file/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="15975" windowHeight="9915" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="555" windowWidth="15975" windowHeight="9915"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -29,13 +29,7 @@
     <t>причина дефекту/невідповідності</t>
   </si>
   <si>
-    <t>кількість ударів при заміні аплікатора</t>
-  </si>
-  <si>
     <t>різниця циклів між замінами</t>
-  </si>
-  <si>
-    <t>Аплікатор</t>
   </si>
   <si>
     <t>**</t>
@@ -45,36 +39,6 @@
   </si>
   <si>
     <t>спрогонозоване середне значення циклів між замінами</t>
-  </si>
-  <si>
-    <t>24/01/2018</t>
-  </si>
-  <si>
-    <t>3012</t>
-  </si>
-  <si>
-    <t>Не відповідне термоусадження</t>
-  </si>
-  <si>
-    <t>інше</t>
-  </si>
-  <si>
-    <t>31/01/2018</t>
-  </si>
-  <si>
-    <t>Зазубрини в місті відрізу контакту</t>
-  </si>
-  <si>
-    <t>07/02/2018</t>
-  </si>
-  <si>
-    <t>Пошкодження поверхні контакту</t>
-  </si>
-  <si>
-    <t>08/02/2018</t>
-  </si>
-  <si>
-    <t>Асиметрія контакту</t>
   </si>
   <si>
     <t>sap #</t>
@@ -89,10 +53,7 @@
     <t>difference cycles</t>
   </si>
   <si>
-    <t>anvil</t>
-  </si>
-  <si>
-    <t>crimper wire</t>
+    <t>кількість ударів при  ремонті</t>
   </si>
 </sst>
 </file>
@@ -330,11 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -353,6 +309,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
@@ -683,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,19 +660,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17">
+      <c r="A1" s="25">
         <v>80000000</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>9</v>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -725,214 +686,147 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="21">
-        <v>320000</v>
-      </c>
-      <c r="I2" s="24"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="1" t="e">
         <f t="shared" ref="E3:E11" si="0">D3-D2</f>
         <v>#VALUE!</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="22"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12">
-        <v>100</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12">
-        <v>200</v>
-      </c>
+      <c r="A5" s="12"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="24"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12">
-        <v>320</v>
-      </c>
+      <c r="A6" s="12"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="12">
-        <v>350</v>
-      </c>
+      <c r="A7" s="12"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1">
         <f>D7-D6</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="12">
-        <v>370</v>
-      </c>
+      <c r="A8" s="12"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12">
-        <v>500</v>
-      </c>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="12">
-        <v>650</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1200</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>0</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" s="1">
-        <f t="shared" ref="E5:E62" si="1">D12-D11</f>
-        <v>-1200</v>
+        <f t="shared" ref="E12:E62" si="1">D12-D11</f>
+        <v>0</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
@@ -940,8 +834,8 @@
         <v>0</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
@@ -949,8 +843,8 @@
         <v>0</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
@@ -958,8 +852,8 @@
         <v>0</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
@@ -967,8 +861,8 @@
         <v>0</v>
       </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
@@ -976,8 +870,8 @@
         <v>0</v>
       </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
@@ -985,8 +879,8 @@
         <v>0</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
@@ -994,8 +888,8 @@
         <v>0</v>
       </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
@@ -1003,8 +897,8 @@
         <v>0</v>
       </c>
       <c r="F20" s="14"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
@@ -1012,8 +906,8 @@
         <v>0</v>
       </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
@@ -1021,8 +915,8 @@
         <v>0</v>
       </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
@@ -1030,8 +924,8 @@
         <v>0</v>
       </c>
       <c r="F23" s="14"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
@@ -1039,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
@@ -1047,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="14"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
@@ -49862,8 +49756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1971" workbookViewId="0">
-      <selection activeCell="J2002" sqref="J2002"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49874,23 +49768,23 @@
     <col min="4" max="4" width="16.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>23</v>
+    <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="11">
         <f>C3-C2</f>
@@ -61783,145 +61677,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1985" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1985" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1985" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1986" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1986" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1986" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1987" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1987" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1987" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1988" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1988" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1988" s="11">
         <f t="shared" ref="D1988:D2000" si="31">C1988-C1987</f>
         <v>0</v>
       </c>
     </row>
-    <row r="1989" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1989" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1989" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1990" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1990" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1990" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1991" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1991" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1991" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1992" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1992" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1992" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1993" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1993" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1993" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1994" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1994" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1994" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1995" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1995" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1995" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1996" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1996" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1996" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1997" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1997" s="11">
-        <v>1</v>
-      </c>
+    <row r="1997" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1997" s="11">
         <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1998" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1998" s="11">
-        <v>400001370</v>
-      </c>
-      <c r="B1998" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1998" s="11">
-        <v>119000</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1998" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1998" s="11">
         <f t="shared" si="31"/>
-        <v>118999</v>
+        <v>0</v>
       </c>
       <c r="E1998" s="12">
         <f>IF(D1998&gt;0,D1998,0)</f>
-        <v>118999</v>
-      </c>
-    </row>
-    <row r="1999" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1999" s="11">
-        <v>400001964</v>
-      </c>
-      <c r="B1999" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1999" s="11">
-        <v>120000</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1999" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1999" s="11">
         <f t="shared" si="31"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E1999">
         <f>IF(D1999&gt;0,D1999,0)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2000" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2000" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D2000" s="11">
         <f t="shared" si="31"/>
-        <v>-120000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2001" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2001" s="27">
+      <c r="A2001" s="24">
         <f>COUNT(A3:A2000)</f>
-        <v>2</v>
-      </c>
-      <c r="B2001" s="27"/>
-      <c r="C2001" s="27"/>
-      <c r="E2001" s="27">
+        <v>0</v>
+      </c>
+      <c r="B2001" s="24"/>
+      <c r="C2001" s="24"/>
+      <c r="E2001" s="24">
         <f>SUM(E3:E2000)</f>
-        <v>119999</v>
-      </c>
-      <c r="F2001">
+        <v>0</v>
+      </c>
+      <c r="F2001" t="e">
         <f>E2001/A2001</f>
-        <v>59999.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add eq files, workin version, need refactoring for good OOP
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/template.xlsx
+++ b/eq_log/eq_file/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="15975" windowHeight="9915" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="555" windowWidth="15975" windowHeight="9915"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -29,13 +29,7 @@
     <t>причина дефекту/невідповідності</t>
   </si>
   <si>
-    <t>кількість ударів при заміні аплікатора</t>
-  </si>
-  <si>
     <t>різниця циклів між замінами</t>
-  </si>
-  <si>
-    <t>Аплікатор</t>
   </si>
   <si>
     <t>**</t>
@@ -45,36 +39,6 @@
   </si>
   <si>
     <t>спрогонозоване середне значення циклів між замінами</t>
-  </si>
-  <si>
-    <t>24/01/2018</t>
-  </si>
-  <si>
-    <t>3012</t>
-  </si>
-  <si>
-    <t>Не відповідне термоусадження</t>
-  </si>
-  <si>
-    <t>інше</t>
-  </si>
-  <si>
-    <t>31/01/2018</t>
-  </si>
-  <si>
-    <t>Зазубрини в місті відрізу контакту</t>
-  </si>
-  <si>
-    <t>07/02/2018</t>
-  </si>
-  <si>
-    <t>Пошкодження поверхні контакту</t>
-  </si>
-  <si>
-    <t>08/02/2018</t>
-  </si>
-  <si>
-    <t>Асиметрія контакту</t>
   </si>
   <si>
     <t>sap #</t>
@@ -89,10 +53,7 @@
     <t>difference cycles</t>
   </si>
   <si>
-    <t>anvil</t>
-  </si>
-  <si>
-    <t>crimper wire</t>
+    <t>кількість ударів при  ремонті</t>
   </si>
 </sst>
 </file>
@@ -330,11 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -353,6 +309,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
@@ -683,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,19 +660,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17">
+      <c r="A1" s="25">
         <v>80000000</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>9</v>
+      <c r="H1" s="17" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -725,214 +686,147 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="21">
-        <v>320000</v>
-      </c>
-      <c r="I2" s="24"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="1" t="e">
         <f t="shared" ref="E3:E11" si="0">D3-D2</f>
         <v>#VALUE!</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="22"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12">
-        <v>100</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12">
-        <v>200</v>
-      </c>
+      <c r="A5" s="12"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="24"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12">
-        <v>320</v>
-      </c>
+      <c r="A6" s="12"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="12">
-        <v>350</v>
-      </c>
+      <c r="A7" s="12"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1">
         <f>D7-D6</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="12">
-        <v>370</v>
-      </c>
+      <c r="A8" s="12"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12">
-        <v>500</v>
-      </c>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="12">
-        <v>650</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1200</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>0</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" s="1">
-        <f t="shared" ref="E5:E62" si="1">D12-D11</f>
-        <v>-1200</v>
+        <f t="shared" ref="E12:E62" si="1">D12-D11</f>
+        <v>0</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
@@ -940,8 +834,8 @@
         <v>0</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
@@ -949,8 +843,8 @@
         <v>0</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
@@ -958,8 +852,8 @@
         <v>0</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
@@ -967,8 +861,8 @@
         <v>0</v>
       </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
@@ -976,8 +870,8 @@
         <v>0</v>
       </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
@@ -985,8 +879,8 @@
         <v>0</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
@@ -994,8 +888,8 @@
         <v>0</v>
       </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
@@ -1003,8 +897,8 @@
         <v>0</v>
       </c>
       <c r="F20" s="14"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
@@ -1012,8 +906,8 @@
         <v>0</v>
       </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
@@ -1021,8 +915,8 @@
         <v>0</v>
       </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
@@ -1030,8 +924,8 @@
         <v>0</v>
       </c>
       <c r="F23" s="14"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
@@ -1039,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
@@ -1047,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="14"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
@@ -49862,8 +49756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1971" workbookViewId="0">
-      <selection activeCell="J2002" sqref="J2002"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49874,23 +49768,23 @@
     <col min="4" max="4" width="16.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>23</v>
+    <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="11">
         <f>C3-C2</f>
@@ -61783,145 +61677,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1985" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1985" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1985" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1986" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1986" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1986" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1987" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1987" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1987" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1988" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1988" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1988" s="11">
         <f t="shared" ref="D1988:D2000" si="31">C1988-C1987</f>
         <v>0</v>
       </c>
     </row>
-    <row r="1989" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1989" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1989" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1990" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1990" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1990" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1991" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1991" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1991" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1992" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1992" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1992" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1993" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1993" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1993" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1994" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1994" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1994" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1995" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1995" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1995" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1996" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1996" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1996" s="11">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="1997" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1997" s="11">
-        <v>1</v>
-      </c>
+    <row r="1997" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1997" s="11">
         <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1998" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1998" s="11">
-        <v>400001370</v>
-      </c>
-      <c r="B1998" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1998" s="11">
-        <v>119000</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1998" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1998" s="11">
         <f t="shared" si="31"/>
-        <v>118999</v>
+        <v>0</v>
       </c>
       <c r="E1998" s="12">
         <f>IF(D1998&gt;0,D1998,0)</f>
-        <v>118999</v>
-      </c>
-    </row>
-    <row r="1999" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1999" s="11">
-        <v>400001964</v>
-      </c>
-      <c r="B1999" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1999" s="11">
-        <v>120000</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1999" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D1999" s="11">
         <f t="shared" si="31"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E1999">
         <f>IF(D1999&gt;0,D1999,0)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2000" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2000" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D2000" s="11">
         <f t="shared" si="31"/>
-        <v>-120000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2001" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2001" s="27">
+      <c r="A2001" s="24">
         <f>COUNT(A3:A2000)</f>
-        <v>2</v>
-      </c>
-      <c r="B2001" s="27"/>
-      <c r="C2001" s="27"/>
-      <c r="E2001" s="27">
+        <v>0</v>
+      </c>
+      <c r="B2001" s="24"/>
+      <c r="C2001" s="24"/>
+      <c r="E2001" s="24">
         <f>SUM(E3:E2000)</f>
-        <v>119999</v>
-      </c>
-      <c r="F2001">
+        <v>0</v>
+      </c>
+      <c r="F2001" t="e">
         <f>E2001/A2001</f>
-        <v>59999.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>